<commit_message>
nearly done with 3A1
</commit_message>
<xml_diff>
--- a/IIA/3A1/Transition_to_turbulence/data.xlsx
+++ b/IIA/3A1/Transition_to_turbulence/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\MEng-CW\IIA\3A1\Transition_to_turbulence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BB1962-A691-476A-9757-9B3F0483CEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47C03CE-1114-490F-926F-0C1BFFBC3B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="preface" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Dial setting</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Uinf</t>
   </si>
   <si>
-    <t>Re</t>
-  </si>
-  <si>
     <t>Obs</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>Turbulent</t>
   </si>
   <si>
-    <t>Fully developed</t>
-  </si>
-  <si>
     <t>Observations from flat plate</t>
   </si>
   <si>
@@ -136,6 +130,54 @@
   </si>
   <si>
     <t>height</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>E_bar</t>
+  </si>
+  <si>
+    <t>E'</t>
+  </si>
+  <si>
+    <t>Ubar</t>
+  </si>
+  <si>
+    <t>U'</t>
+  </si>
+  <si>
+    <t>Re_x</t>
+  </si>
+  <si>
+    <t>dt_spot ms</t>
+  </si>
+  <si>
+    <t>dt_peak ms</t>
+  </si>
+  <si>
+    <t>spot size</t>
+  </si>
+  <si>
+    <t>eddy size</t>
+  </si>
+  <si>
+    <t>DIAL</t>
+  </si>
+  <si>
+    <t>Flat plate</t>
+  </si>
+  <si>
+    <t>Protrusion</t>
+  </si>
+  <si>
+    <t>Trip wire</t>
+  </si>
+  <si>
+    <t>setup</t>
+  </si>
+  <si>
+    <t>eddy size mm</t>
   </si>
 </sst>
 </file>
@@ -253,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -270,6 +312,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1533,20 +1580,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="8" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>13</v>
       </c>
@@ -1554,13 +1604,13 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1571,16 +1621,16 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E4">
         <v>1.2250000000000001</v>
       </c>
@@ -1591,7 +1641,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -1599,7 +1649,7 @@
         <v>1.5898670142424867</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -1607,33 +1657,57 @@
         <v>0.59689403804214392</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>300</v>
       </c>
@@ -1648,11 +1722,25 @@
         <f>$E$4*D13*$G$4/$F$4</f>
         <v>399873.4049123202</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f>((J13^2-$C$7)/$C$8)^2</f>
+        <v>1.4145108282113836</v>
+      </c>
+      <c r="G13">
+        <f>0.001*K13*4*J13*(J13^2-$C$7)/$C$8^2</f>
+        <v>8.1923758302220318E-2</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13">
+        <v>1.5165</v>
+      </c>
+      <c r="K13">
+        <v>6.7779999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>650</v>
       </c>
@@ -1667,11 +1755,40 @@
         <f t="shared" ref="E14:E16" si="1">$E$4*D14*$G$4/$F$4</f>
         <v>1229540.5259852866</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" ref="F14:F16" si="2">((J14^2-$C$7)/$C$8)^2</f>
+        <v>7.9021272816272736</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G26" si="3">0.001*K14*4*J14*(J14^2-$C$7)/$C$8^2</f>
+        <v>0.77505652418517978</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>1.8077000000000001</v>
+      </c>
+      <c r="K14">
+        <v>22.76</v>
+      </c>
+      <c r="L14">
+        <v>25</v>
+      </c>
+      <c r="M14" s="15">
+        <f>L14/4</f>
+        <v>6.25</v>
+      </c>
+      <c r="N14">
+        <f>L14*F14/1000</f>
+        <v>0.19755318204068184</v>
+      </c>
+      <c r="O14">
+        <f>M14*G14/1000</f>
+        <v>4.8441032761573737E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>820</v>
       </c>
@@ -1686,11 +1803,41 @@
         <f t="shared" si="1"/>
         <v>1520284.053991568</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>11.066357720989568</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>5.0554695414118103E-3</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15">
+        <v>1.8909</v>
+      </c>
+      <c r="K15">
+        <v>0.11992999999999999</v>
+      </c>
+      <c r="L15">
+        <f>8*25</f>
+        <v>200</v>
+      </c>
+      <c r="M15">
+        <f>L15/24</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="N15">
+        <f t="shared" ref="N15:N21" si="4">L15*F15/1000</f>
+        <v>2.2132715441979136</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ref="O15:O26" si="5">M15*G15/1000</f>
+        <v>4.2128912845098421E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="8">
         <v>1000</v>
       </c>
@@ -1705,21 +1852,46 @@
         <f t="shared" si="1"/>
         <v>1747172.6612599567</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>13.252804539076868</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>0.5953251674052169</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16">
+        <v>1.9398</v>
+      </c>
+      <c r="K16">
+        <v>12.58</v>
+      </c>
+      <c r="L16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16">
+        <f>100/20</f>
+        <v>5</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="5"/>
+        <v>2.9766258370260844E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
-        <v>25</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>300</v>
       </c>
@@ -1727,18 +1899,32 @@
         <v>0.11</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20:D22" si="2">SQRT(2*100*C20/$E$4)</f>
+        <f t="shared" ref="D20:D22" si="6">SQRT(2*100*C20/$E$4)</f>
         <v>4.2378277069118075</v>
       </c>
       <c r="E20" s="4">
         <f>$E$4*D20*$G$4/$F$4</f>
         <v>399873.4049123202</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" ref="F20:F22" si="7">((J20^2-$C$7)/$C$8)^2</f>
+        <v>1.6103816711412877</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>0.26000863275777802</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20">
+        <v>1.5321</v>
+      </c>
+      <c r="K20">
+        <v>19.956</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <v>370</v>
       </c>
@@ -1746,18 +1932,48 @@
         <v>0.34</v>
       </c>
       <c r="D21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>7.4505170345173131</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" ref="E21:E22" si="3">$E$4*D21*$G$4/$F$4</f>
+        <f t="shared" ref="E21:E22" si="8">$E$4*D21*$G$4/$F$4</f>
         <v>703016.69180428563</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <f t="shared" si="7"/>
+        <v>3.5194073061705042</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>0.67654271368132024</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21">
+        <v>1.6460999999999999</v>
+      </c>
+      <c r="K21">
+        <v>32.692</v>
+      </c>
+      <c r="L21">
+        <f>1.7 *25</f>
+        <v>42.5</v>
+      </c>
+      <c r="M21">
+        <f>L21/6</f>
+        <v>7.083333333333333</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="4"/>
+        <v>0.14957481051224644</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="5"/>
+        <v>4.7921775552426842E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="8">
         <v>430</v>
       </c>
@@ -1765,28 +1981,50 @@
         <v>0.47</v>
       </c>
       <c r="D22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>8.7598341238605091</v>
       </c>
       <c r="E22" s="6">
+        <f t="shared" si="8"/>
+        <v>826561.37526832428</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="7"/>
+        <v>5.177820972544934</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="3"/>
-        <v>826561.37526832428</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.67691526053782225</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22">
+        <v>1.7170000000000001</v>
+      </c>
+      <c r="K22">
+        <v>25.853999999999999</v>
+      </c>
+      <c r="M22">
+        <f>100/14</f>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="5"/>
+        <v>4.8351090038415874E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="8">
         <v>200</v>
       </c>
@@ -1794,24 +2032,193 @@
         <v>0.04</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26" si="4">SQRT(2*100*C26/$E$4)</f>
+        <f t="shared" ref="D26" si="9">SQRT(2*100*C26/$E$4)</f>
         <v>2.5555062599997593</v>
       </c>
       <c r="E26" s="6">
-        <f t="shared" ref="E26" si="5">$E$4*D26*$G$4/$F$4</f>
+        <f t="shared" ref="E26" si="10">$E$4*D26*$G$4/$F$4</f>
         <v>241132.73595200432</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="F26">
+        <f t="shared" ref="F26" si="11">((J26^2-$C$7)/$C$8)^2</f>
+        <v>1.1585325608202335</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>0.58546948920544728</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26">
+        <v>1.4941</v>
+      </c>
+      <c r="K26">
+        <v>54.326000000000001</v>
+      </c>
+      <c r="M26">
+        <f>200/12</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="5"/>
+        <v>9.7578248200907887E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="7">
+        <v>650</v>
+      </c>
+      <c r="D32">
+        <v>25</v>
+      </c>
+      <c r="E32" s="15">
+        <f>D32/4</f>
+        <v>6.25</v>
+      </c>
+      <c r="F32">
+        <f>D32*F13</f>
+        <v>35.362770705284589</v>
+      </c>
+      <c r="G32">
+        <f>E32*G14</f>
+        <v>4.8441032761573739</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="16"/>
+      <c r="C33" s="7">
+        <v>820</v>
+      </c>
+      <c r="D33">
+        <f>8*25</f>
+        <v>200</v>
+      </c>
+      <c r="E33">
+        <f>D33/24</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="F33">
+        <f>D33*F14</f>
+        <v>1580.4254563254547</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ref="G33:G39" si="12">E33*G15</f>
+        <v>4.2128912845098419E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="16"/>
+      <c r="C34" s="8">
+        <v>1000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34">
+        <f>100/20</f>
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="12"/>
+        <v>2.9766258370260843</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="7">
+        <v>370</v>
+      </c>
+      <c r="D36">
+        <f>1.7 *25</f>
+        <v>42.5</v>
+      </c>
+      <c r="E36">
+        <f>D36/6</f>
+        <v>7.083333333333333</v>
+      </c>
+      <c r="F36">
+        <f>D36*G21</f>
+        <v>28.75306533145611</v>
+      </c>
+      <c r="G36">
+        <f>E36*G21</f>
+        <v>4.7921775552426844</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="16"/>
+      <c r="C37" s="8">
+        <v>430</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37">
+        <f>100/14</f>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="G37">
+        <f>E37*G22</f>
+        <v>4.8351090038415876</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="8">
+        <v>200</v>
+      </c>
+      <c r="D39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39">
+        <f>200/12</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="G39">
+        <f>E39*G26</f>
+        <v>9.7578248200907893</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="B36:B37"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B32:B34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>